<commit_message>
Add spring demo bike list check.
</commit_message>
<xml_diff>
--- a/proj02_springdemo/data/SpringDemo-MarketMatrix-20190517.xlsx
+++ b/proj02_springdemo/data/SpringDemo-MarketMatrix-20190517.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents\HD\Spring Demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\bitbucket\hd-emea-test-script\proj02_springdemo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="279">
   <si>
     <t>Softail</t>
   </si>
@@ -804,13 +804,79 @@
   </si>
   <si>
     <t>Ultra Limited</t>
+  </si>
+  <si>
+    <t>FXBB</t>
+  </si>
+  <si>
+    <t>FLFB</t>
+  </si>
+  <si>
+    <t>FLSB</t>
+  </si>
+  <si>
+    <t>FLHC</t>
+  </si>
+  <si>
+    <t>FXFB</t>
+  </si>
+  <si>
+    <t>FXDRS</t>
+  </si>
+  <si>
+    <t>FXBR</t>
+  </si>
+  <si>
+    <t>FLSL</t>
+  </si>
+  <si>
+    <t>FLDE</t>
+  </si>
+  <si>
+    <t>FXLR</t>
+  </si>
+  <si>
+    <t>XL883N</t>
+  </si>
+  <si>
+    <t>XL1200NS</t>
+  </si>
+  <si>
+    <t>XL1200X</t>
+  </si>
+  <si>
+    <t>XL1200XS</t>
+  </si>
+  <si>
+    <t>XL1200CX</t>
+  </si>
+  <si>
+    <t>FLHRXS</t>
+  </si>
+  <si>
+    <t>FLHXS</t>
+  </si>
+  <si>
+    <t>FLTRXS</t>
+  </si>
+  <si>
+    <t>FLTRU</t>
+  </si>
+  <si>
+    <t>FLHTK</t>
+  </si>
+  <si>
+    <t>XG750</t>
+  </si>
+  <si>
+    <t>XG750A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -947,6 +1013,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -2006,7 +2078,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="274">
+  <cellXfs count="275">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2638,100 +2710,7 @@
     <xf numFmtId="16" fontId="11" fillId="11" borderId="59" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2758,12 +2737,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="68" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="65" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2819,6 +2792,106 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="74" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="54" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="68" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3154,11 +3227,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="10" ySplit="4" topLeftCell="K5" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="10" ySplit="4" topLeftCell="K17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3167,12 +3240,12 @@
     <col min="2" max="3" width="12.28515625" style="1"/>
     <col min="4" max="4" width="22.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="19" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" style="83" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="39.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28.5703125" style="83" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="31.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="21.42578125" style="1" customWidth="1"/>
     <col min="13" max="13" width="25.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="25.140625" style="29" customWidth="1"/>
@@ -3182,7 +3255,7 @@
     <col min="36" max="36" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="23.28515625" style="82" customWidth="1"/>
     <col min="38" max="38" width="23.28515625" style="1" customWidth="1"/>
-    <col min="39" max="39" width="23.28515625" style="34" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="26.85546875" style="34" customWidth="1"/>
     <col min="40" max="40" width="62.140625" style="1" customWidth="1"/>
     <col min="41" max="41" width="65" style="1" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="50.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -3190,7 +3263,7 @@
     <col min="44" max="16384" width="12.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="29" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" s="29" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="84"/>
       <c r="B1" s="84"/>
       <c r="C1" s="84"/>
@@ -3202,33 +3275,87 @@
       <c r="I1" s="84"/>
       <c r="J1" s="84"/>
       <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="181"/>
-      <c r="Q1" s="181"/>
-      <c r="R1" s="181"/>
-      <c r="S1" s="181"/>
-      <c r="T1" s="181"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
-      <c r="AG1" s="84"/>
-      <c r="AH1" s="84"/>
-      <c r="AI1" s="84"/>
-      <c r="AJ1" s="84"/>
-      <c r="AK1" s="84"/>
-      <c r="AL1" s="84"/>
+      <c r="L1" s="241" t="s">
+        <v>257</v>
+      </c>
+      <c r="M1" s="241" t="s">
+        <v>258</v>
+      </c>
+      <c r="N1" s="241" t="s">
+        <v>259</v>
+      </c>
+      <c r="O1" s="241" t="s">
+        <v>260</v>
+      </c>
+      <c r="P1" s="241" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q1" s="241" t="s">
+        <v>273</v>
+      </c>
+      <c r="R1" s="241" t="s">
+        <v>274</v>
+      </c>
+      <c r="S1" s="241" t="s">
+        <v>275</v>
+      </c>
+      <c r="T1" s="241" t="s">
+        <v>276</v>
+      </c>
+      <c r="U1" s="241" t="s">
+        <v>262</v>
+      </c>
+      <c r="V1" s="241" t="s">
+        <v>261</v>
+      </c>
+      <c r="W1" s="241" t="s">
+        <v>263</v>
+      </c>
+      <c r="X1" s="241" t="s">
+        <v>264</v>
+      </c>
+      <c r="Y1" s="241" t="s">
+        <v>265</v>
+      </c>
+      <c r="Z1" s="241" t="s">
+        <v>266</v>
+      </c>
+      <c r="AA1" s="241" t="s">
+        <v>277</v>
+      </c>
+      <c r="AB1" s="241" t="s">
+        <v>278</v>
+      </c>
+      <c r="AC1" s="241" t="s">
+        <v>267</v>
+      </c>
+      <c r="AD1" s="241" t="s">
+        <v>268</v>
+      </c>
+      <c r="AE1" s="241" t="s">
+        <v>269</v>
+      </c>
+      <c r="AF1" s="241" t="s">
+        <v>270</v>
+      </c>
+      <c r="AG1" s="241" t="s">
+        <v>271</v>
+      </c>
+      <c r="AH1" s="241" t="s">
+        <v>257</v>
+      </c>
+      <c r="AI1" s="241" t="s">
+        <v>259</v>
+      </c>
+      <c r="AJ1" s="241" t="s">
+        <v>261</v>
+      </c>
+      <c r="AK1" s="241" t="s">
+        <v>258</v>
+      </c>
+      <c r="AL1" s="241" t="s">
+        <v>262</v>
+      </c>
       <c r="AM1" s="84"/>
       <c r="AN1" s="84"/>
       <c r="AO1" s="84"/>
@@ -3244,43 +3371,43 @@
       <c r="I2" s="84"/>
       <c r="J2" s="84"/>
       <c r="K2" s="84"/>
-      <c r="L2" s="225" t="s">
+      <c r="L2" s="256" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="226"/>
-      <c r="N2" s="226"/>
-      <c r="O2" s="226"/>
-      <c r="P2" s="226"/>
-      <c r="Q2" s="226"/>
-      <c r="R2" s="226"/>
-      <c r="S2" s="226"/>
-      <c r="T2" s="226"/>
-      <c r="U2" s="226"/>
-      <c r="V2" s="226"/>
-      <c r="W2" s="226"/>
-      <c r="X2" s="226"/>
-      <c r="Y2" s="226"/>
-      <c r="Z2" s="227"/>
-      <c r="AA2" s="219" t="s">
+      <c r="M2" s="257"/>
+      <c r="N2" s="257"/>
+      <c r="O2" s="257"/>
+      <c r="P2" s="257"/>
+      <c r="Q2" s="257"/>
+      <c r="R2" s="257"/>
+      <c r="S2" s="257"/>
+      <c r="T2" s="257"/>
+      <c r="U2" s="257"/>
+      <c r="V2" s="257"/>
+      <c r="W2" s="257"/>
+      <c r="X2" s="257"/>
+      <c r="Y2" s="257"/>
+      <c r="Z2" s="258"/>
+      <c r="AA2" s="250" t="s">
         <v>1</v>
       </c>
-      <c r="AB2" s="220"/>
-      <c r="AC2" s="220"/>
-      <c r="AD2" s="220"/>
-      <c r="AE2" s="220"/>
-      <c r="AF2" s="220"/>
-      <c r="AG2" s="220"/>
-      <c r="AH2" s="220"/>
-      <c r="AI2" s="220"/>
-      <c r="AJ2" s="220"/>
-      <c r="AK2" s="220"/>
-      <c r="AL2" s="221"/>
+      <c r="AB2" s="251"/>
+      <c r="AC2" s="251"/>
+      <c r="AD2" s="251"/>
+      <c r="AE2" s="251"/>
+      <c r="AF2" s="251"/>
+      <c r="AG2" s="251"/>
+      <c r="AH2" s="251"/>
+      <c r="AI2" s="251"/>
+      <c r="AJ2" s="251"/>
+      <c r="AK2" s="251"/>
+      <c r="AL2" s="252"/>
       <c r="AM2" s="36"/>
       <c r="AN2" s="84"/>
       <c r="AO2" s="84"/>
       <c r="AQ2" s="84"/>
     </row>
-    <row r="3" spans="1:43" s="29" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:43" s="29" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="84"/>
       <c r="B3" s="84"/>
       <c r="C3" s="84"/>
@@ -3292,48 +3419,48 @@
       <c r="I3" s="84"/>
       <c r="J3" s="84"/>
       <c r="K3" s="84"/>
-      <c r="L3" s="228" t="s">
+      <c r="L3" s="259" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="229"/>
-      <c r="N3" s="230" t="s">
+      <c r="M3" s="260"/>
+      <c r="N3" s="261" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="231"/>
-      <c r="P3" s="231"/>
-      <c r="Q3" s="231"/>
-      <c r="R3" s="231"/>
-      <c r="S3" s="231"/>
-      <c r="T3" s="229"/>
-      <c r="U3" s="230" t="s">
+      <c r="O3" s="262"/>
+      <c r="P3" s="262"/>
+      <c r="Q3" s="262"/>
+      <c r="R3" s="262"/>
+      <c r="S3" s="262"/>
+      <c r="T3" s="260"/>
+      <c r="U3" s="261" t="s">
         <v>4</v>
       </c>
-      <c r="V3" s="229"/>
-      <c r="W3" s="230" t="s">
+      <c r="V3" s="260"/>
+      <c r="W3" s="261" t="s">
         <v>5</v>
       </c>
-      <c r="X3" s="231"/>
-      <c r="Y3" s="231"/>
-      <c r="Z3" s="232"/>
-      <c r="AA3" s="222"/>
-      <c r="AB3" s="223"/>
-      <c r="AC3" s="223"/>
-      <c r="AD3" s="223"/>
-      <c r="AE3" s="223"/>
-      <c r="AF3" s="223"/>
-      <c r="AG3" s="223"/>
-      <c r="AH3" s="223"/>
-      <c r="AI3" s="223"/>
-      <c r="AJ3" s="223"/>
-      <c r="AK3" s="223"/>
-      <c r="AL3" s="224"/>
+      <c r="X3" s="262"/>
+      <c r="Y3" s="262"/>
+      <c r="Z3" s="263"/>
+      <c r="AA3" s="253"/>
+      <c r="AB3" s="254"/>
+      <c r="AC3" s="254"/>
+      <c r="AD3" s="254"/>
+      <c r="AE3" s="254"/>
+      <c r="AF3" s="254"/>
+      <c r="AG3" s="254"/>
+      <c r="AH3" s="254"/>
+      <c r="AI3" s="254"/>
+      <c r="AJ3" s="254"/>
+      <c r="AK3" s="254"/>
+      <c r="AL3" s="255"/>
       <c r="AM3" s="36"/>
       <c r="AN3" s="84"/>
       <c r="AO3" s="84"/>
       <c r="AP3" s="84"/>
       <c r="AQ3" s="84"/>
     </row>
-    <row r="4" spans="1:43" s="30" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:43" s="30" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="33" t="s">
         <v>6</v>
       </c>
@@ -3370,19 +3497,19 @@
       <c r="O4" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="242" t="s">
+      <c r="P4" s="213" t="s">
         <v>252</v>
       </c>
-      <c r="Q4" s="242" t="s">
+      <c r="Q4" s="213" t="s">
         <v>253</v>
       </c>
-      <c r="R4" s="242" t="s">
+      <c r="R4" s="213" t="s">
         <v>254</v>
       </c>
-      <c r="S4" s="242" t="s">
+      <c r="S4" s="213" t="s">
         <v>255</v>
       </c>
-      <c r="T4" s="242" t="s">
+      <c r="T4" s="213" t="s">
         <v>256</v>
       </c>
       <c r="U4" s="35" t="s">
@@ -3454,10 +3581,10 @@
     </row>
     <row r="5" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="84"/>
-      <c r="B5" s="233" t="s">
+      <c r="B5" s="264" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="234"/>
+      <c r="C5" s="265"/>
       <c r="D5" s="87" t="s">
         <v>39</v>
       </c>
@@ -3545,8 +3672,8 @@
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="84"/>
-      <c r="B6" s="235"/>
-      <c r="C6" s="236"/>
+      <c r="B6" s="266"/>
+      <c r="C6" s="267"/>
       <c r="D6" s="88" t="s">
         <v>48</v>
       </c>
@@ -3632,8 +3759,8 @@
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="84"/>
-      <c r="B7" s="235"/>
-      <c r="C7" s="236"/>
+      <c r="B7" s="266"/>
+      <c r="C7" s="267"/>
       <c r="D7" s="88" t="s">
         <v>57</v>
       </c>
@@ -3719,8 +3846,8 @@
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="84"/>
-      <c r="B8" s="235"/>
-      <c r="C8" s="236"/>
+      <c r="B8" s="266"/>
+      <c r="C8" s="267"/>
       <c r="D8" s="88" t="s">
         <v>61</v>
       </c>
@@ -3806,8 +3933,8 @@
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" s="84"/>
-      <c r="B9" s="235"/>
-      <c r="C9" s="236"/>
+      <c r="B9" s="266"/>
+      <c r="C9" s="267"/>
       <c r="D9" s="89" t="s">
         <v>64</v>
       </c>
@@ -3893,8 +4020,8 @@
     </row>
     <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" s="84"/>
-      <c r="B10" s="235"/>
-      <c r="C10" s="236"/>
+      <c r="B10" s="266"/>
+      <c r="C10" s="267"/>
       <c r="D10" s="89" t="s">
         <v>67</v>
       </c>
@@ -3978,10 +4105,10 @@
       <c r="AP10" s="24"/>
       <c r="AQ10" s="84"/>
     </row>
-    <row r="11" spans="1:43" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:43" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="84"/>
-      <c r="B11" s="235"/>
-      <c r="C11" s="236"/>
+      <c r="B11" s="266"/>
+      <c r="C11" s="267"/>
       <c r="D11" s="90" t="s">
         <v>70</v>
       </c>
@@ -4073,8 +4200,8 @@
     </row>
     <row r="12" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="84"/>
-      <c r="B12" s="235"/>
-      <c r="C12" s="236"/>
+      <c r="B12" s="266"/>
+      <c r="C12" s="267"/>
       <c r="D12" s="90" t="s">
         <v>77</v>
       </c>
@@ -4164,8 +4291,8 @@
     </row>
     <row r="13" spans="1:43" s="71" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="84"/>
-      <c r="B13" s="235"/>
-      <c r="C13" s="236"/>
+      <c r="B13" s="266"/>
+      <c r="C13" s="267"/>
       <c r="D13" s="90" t="s">
         <v>83</v>
       </c>
@@ -4251,8 +4378,8 @@
     </row>
     <row r="14" spans="1:43" s="71" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="84"/>
-      <c r="B14" s="235"/>
-      <c r="C14" s="236"/>
+      <c r="B14" s="266"/>
+      <c r="C14" s="267"/>
       <c r="D14" s="90" t="s">
         <v>86</v>
       </c>
@@ -4336,10 +4463,10 @@
       <c r="AP14" s="78"/>
       <c r="AQ14" s="84"/>
     </row>
-    <row r="15" spans="1:43" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="84"/>
-      <c r="B15" s="235"/>
-      <c r="C15" s="236"/>
+      <c r="B15" s="266"/>
+      <c r="C15" s="267"/>
       <c r="D15" s="90" t="s">
         <v>88</v>
       </c>
@@ -4429,8 +4556,8 @@
     </row>
     <row r="16" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="84"/>
-      <c r="B16" s="237"/>
-      <c r="C16" s="239"/>
+      <c r="B16" s="268"/>
+      <c r="C16" s="270"/>
       <c r="D16" s="91" t="s">
         <v>95</v>
       </c>
@@ -4520,10 +4647,10 @@
     </row>
     <row r="17" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="84"/>
-      <c r="B17" s="233" t="s">
+      <c r="B17" s="264" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="234"/>
+      <c r="C17" s="265"/>
       <c r="D17" s="168" t="s">
         <v>105</v>
       </c>
@@ -4601,8 +4728,8 @@
     </row>
     <row r="18" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="84"/>
-      <c r="B18" s="235"/>
-      <c r="C18" s="236"/>
+      <c r="B18" s="266"/>
+      <c r="C18" s="267"/>
       <c r="D18" s="68" t="s">
         <v>110</v>
       </c>
@@ -4687,8 +4814,8 @@
       <c r="AQ18" s="84"/>
     </row>
     <row r="19" spans="1:43" s="22" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="235"/>
-      <c r="C19" s="236"/>
+      <c r="B19" s="266"/>
+      <c r="C19" s="267"/>
       <c r="D19" s="68" t="s">
         <v>112</v>
       </c>
@@ -4771,8 +4898,8 @@
     </row>
     <row r="20" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="84"/>
-      <c r="B20" s="235"/>
-      <c r="C20" s="236"/>
+      <c r="B20" s="266"/>
+      <c r="C20" s="267"/>
       <c r="D20" s="126" t="s">
         <v>118</v>
       </c>
@@ -4864,8 +4991,8 @@
     </row>
     <row r="21" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="84"/>
-      <c r="B21" s="235"/>
-      <c r="C21" s="236"/>
+      <c r="B21" s="266"/>
+      <c r="C21" s="267"/>
       <c r="D21" s="69" t="s">
         <v>128</v>
       </c>
@@ -4953,8 +5080,8 @@
     </row>
     <row r="22" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="84"/>
-      <c r="B22" s="235"/>
-      <c r="C22" s="236"/>
+      <c r="B22" s="266"/>
+      <c r="C22" s="267"/>
       <c r="D22" s="68" t="s">
         <v>132</v>
       </c>
@@ -5044,8 +5171,8 @@
     </row>
     <row r="23" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="84"/>
-      <c r="B23" s="235"/>
-      <c r="C23" s="236"/>
+      <c r="B23" s="266"/>
+      <c r="C23" s="267"/>
       <c r="D23" s="68" t="s">
         <v>138</v>
       </c>
@@ -5135,8 +5262,8 @@
     </row>
     <row r="24" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="84"/>
-      <c r="B24" s="235"/>
-      <c r="C24" s="236"/>
+      <c r="B24" s="266"/>
+      <c r="C24" s="267"/>
       <c r="D24" s="68" t="s">
         <v>144</v>
       </c>
@@ -5224,10 +5351,10 @@
       </c>
       <c r="AQ24" s="84"/>
     </row>
-    <row r="25" spans="1:43" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:43" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="140"/>
-      <c r="B25" s="237"/>
-      <c r="C25" s="238"/>
+      <c r="B25" s="268"/>
+      <c r="C25" s="269"/>
       <c r="D25" s="70" t="s">
         <v>150</v>
       </c>
@@ -5309,10 +5436,10 @@
       <c r="AP25" s="27"/>
       <c r="AQ25" s="84"/>
     </row>
-    <row r="26" spans="1:43" s="22" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="158"/>
-      <c r="B26" s="233"/>
-      <c r="C26" s="240"/>
+      <c r="B26" s="264"/>
+      <c r="C26" s="271"/>
       <c r="D26" s="190" t="s">
         <v>102</v>
       </c>
@@ -5397,10 +5524,10 @@
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A27" s="84"/>
-      <c r="B27" s="213" t="s">
+      <c r="B27" s="242" t="s">
         <v>154</v>
       </c>
-      <c r="C27" s="214"/>
+      <c r="C27" s="243"/>
       <c r="D27" s="146" t="s">
         <v>155</v>
       </c>
@@ -5488,8 +5615,8 @@
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" s="84"/>
-      <c r="B28" s="215"/>
-      <c r="C28" s="216"/>
+      <c r="B28" s="244"/>
+      <c r="C28" s="245"/>
       <c r="D28" s="51" t="s">
         <v>155</v>
       </c>
@@ -5577,8 +5704,8 @@
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" s="84"/>
-      <c r="B29" s="215"/>
-      <c r="C29" s="216"/>
+      <c r="B29" s="244"/>
+      <c r="C29" s="245"/>
       <c r="D29" s="51" t="s">
         <v>162</v>
       </c>
@@ -5664,8 +5791,8 @@
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" s="84"/>
-      <c r="B30" s="215"/>
-      <c r="C30" s="216"/>
+      <c r="B30" s="244"/>
+      <c r="C30" s="245"/>
       <c r="D30" s="51" t="s">
         <v>167</v>
       </c>
@@ -5751,8 +5878,8 @@
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31" s="84"/>
-      <c r="B31" s="215"/>
-      <c r="C31" s="216"/>
+      <c r="B31" s="244"/>
+      <c r="C31" s="245"/>
       <c r="D31" s="51" t="s">
         <v>169</v>
       </c>
@@ -5838,8 +5965,8 @@
     </row>
     <row r="32" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A32" s="84"/>
-      <c r="B32" s="215"/>
-      <c r="C32" s="216"/>
+      <c r="B32" s="244"/>
+      <c r="C32" s="245"/>
       <c r="D32" s="51" t="s">
         <v>169</v>
       </c>
@@ -5925,8 +6052,8 @@
     </row>
     <row r="33" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A33" s="84"/>
-      <c r="B33" s="215"/>
-      <c r="C33" s="216"/>
+      <c r="B33" s="244"/>
+      <c r="C33" s="245"/>
       <c r="D33" s="51" t="s">
         <v>169</v>
       </c>
@@ -6012,8 +6139,8 @@
     </row>
     <row r="34" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A34" s="84"/>
-      <c r="B34" s="215"/>
-      <c r="C34" s="216"/>
+      <c r="B34" s="244"/>
+      <c r="C34" s="245"/>
       <c r="D34" s="51" t="s">
         <v>175</v>
       </c>
@@ -6101,8 +6228,8 @@
     </row>
     <row r="35" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A35" s="84"/>
-      <c r="B35" s="215"/>
-      <c r="C35" s="216"/>
+      <c r="B35" s="244"/>
+      <c r="C35" s="245"/>
       <c r="D35" s="51" t="s">
         <v>175</v>
       </c>
@@ -6190,8 +6317,8 @@
     </row>
     <row r="36" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A36" s="84"/>
-      <c r="B36" s="215"/>
-      <c r="C36" s="216"/>
+      <c r="B36" s="244"/>
+      <c r="C36" s="245"/>
       <c r="D36" s="51" t="s">
         <v>181</v>
       </c>
@@ -6279,8 +6406,8 @@
     </row>
     <row r="37" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A37" s="84"/>
-      <c r="B37" s="215"/>
-      <c r="C37" s="216"/>
+      <c r="B37" s="244"/>
+      <c r="C37" s="245"/>
       <c r="D37" s="51" t="s">
         <v>183</v>
       </c>
@@ -6367,8 +6494,8 @@
       <c r="AQ37" s="84"/>
     </row>
     <row r="38" spans="1:43" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="215"/>
-      <c r="C38" s="216"/>
+      <c r="B38" s="244"/>
+      <c r="C38" s="245"/>
       <c r="D38" s="52" t="s">
         <v>186</v>
       </c>
@@ -6450,8 +6577,8 @@
       <c r="AP38" s="14"/>
     </row>
     <row r="39" spans="1:43" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="215"/>
-      <c r="C39" s="216"/>
+      <c r="B39" s="244"/>
+      <c r="C39" s="245"/>
       <c r="D39" s="52" t="s">
         <v>189</v>
       </c>
@@ -6533,8 +6660,8 @@
       <c r="AP39" s="14"/>
     </row>
     <row r="40" spans="1:43" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="215"/>
-      <c r="C40" s="216"/>
+      <c r="B40" s="244"/>
+      <c r="C40" s="245"/>
       <c r="D40" s="161" t="s">
         <v>192</v>
       </c>
@@ -6619,8 +6746,8 @@
     </row>
     <row r="41" spans="1:43" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="84"/>
-      <c r="B41" s="217"/>
-      <c r="C41" s="218"/>
+      <c r="B41" s="246"/>
+      <c r="C41" s="247"/>
       <c r="D41" s="197" t="s">
         <v>197</v>
       </c>
@@ -6705,10 +6832,10 @@
       <c r="AQ41" s="84"/>
     </row>
     <row r="42" spans="1:43" s="180" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="241" t="s">
+      <c r="B42" s="272" t="s">
         <v>202</v>
       </c>
-      <c r="C42" s="214"/>
+      <c r="C42" s="243"/>
       <c r="D42" s="182" t="s">
         <v>228</v>
       </c>
@@ -6796,8 +6923,8 @@
       </c>
     </row>
     <row r="43" spans="1:43" s="180" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="215"/>
-      <c r="C43" s="216"/>
+      <c r="B43" s="244"/>
+      <c r="C43" s="245"/>
       <c r="D43" s="186" t="s">
         <v>238</v>
       </c>
@@ -6881,8 +7008,8 @@
       <c r="AP43" s="4"/>
     </row>
     <row r="44" spans="1:43" s="180" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="215"/>
-      <c r="C44" s="216"/>
+      <c r="B44" s="244"/>
+      <c r="C44" s="245"/>
       <c r="D44" s="186" t="s">
         <v>242</v>
       </c>
@@ -6968,30 +7095,30 @@
       <c r="AP44" s="178"/>
     </row>
     <row r="45" spans="1:43" s="180" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="243"/>
-      <c r="C45" s="244"/>
-      <c r="D45" s="245" t="s">
+      <c r="B45" s="273"/>
+      <c r="C45" s="274"/>
+      <c r="D45" s="214" t="s">
         <v>247</v>
       </c>
-      <c r="E45" s="246" t="s">
+      <c r="E45" s="215" t="s">
         <v>248</v>
       </c>
-      <c r="F45" s="247" t="s">
+      <c r="F45" s="216" t="s">
         <v>249</v>
       </c>
-      <c r="G45" s="248" t="s">
+      <c r="G45" s="217" t="s">
         <v>231</v>
       </c>
-      <c r="H45" s="249" t="s">
+      <c r="H45" s="218" t="s">
         <v>226</v>
       </c>
-      <c r="I45" s="249" t="s">
+      <c r="I45" s="218" t="s">
         <v>232</v>
       </c>
-      <c r="J45" s="249" t="s">
+      <c r="J45" s="218" t="s">
         <v>233</v>
       </c>
-      <c r="K45" s="247" t="s">
+      <c r="K45" s="216" t="s">
         <v>234</v>
       </c>
       <c r="L45" s="111" t="s">
@@ -7003,7 +7130,7 @@
       <c r="N45" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="O45" s="250" t="s">
+      <c r="O45" s="219" t="s">
         <v>52</v>
       </c>
       <c r="P45" s="111" t="s">
@@ -7043,46 +7170,46 @@
       <c r="AJ45" s="160"/>
       <c r="AK45" s="160"/>
       <c r="AL45" s="160"/>
-      <c r="AM45" s="251" t="s">
+      <c r="AM45" s="220" t="s">
         <v>73</v>
       </c>
-      <c r="AN45" s="252" t="s">
+      <c r="AN45" s="221" t="s">
         <v>250</v>
       </c>
-      <c r="AO45" s="252"/>
+      <c r="AO45" s="221"/>
       <c r="AP45" s="61"/>
     </row>
     <row r="46" spans="1:43" s="84" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="140"/>
-      <c r="B46" s="253" t="s">
+      <c r="B46" s="248" t="s">
         <v>251</v>
       </c>
-      <c r="C46" s="254"/>
-      <c r="D46" s="255" t="s">
+      <c r="C46" s="249"/>
+      <c r="D46" s="222" t="s">
         <v>203</v>
       </c>
-      <c r="E46" s="256" t="s">
+      <c r="E46" s="223" t="s">
         <v>204</v>
       </c>
-      <c r="F46" s="257" t="s">
+      <c r="F46" s="224" t="s">
         <v>205</v>
       </c>
-      <c r="G46" s="258" t="s">
+      <c r="G46" s="225" t="s">
         <v>206</v>
       </c>
-      <c r="H46" s="258" t="s">
+      <c r="H46" s="225" t="s">
         <v>207</v>
       </c>
-      <c r="I46" s="259" t="s">
+      <c r="I46" s="226" t="s">
         <v>72</v>
       </c>
-      <c r="J46" s="260" t="s">
+      <c r="J46" s="227" t="s">
         <v>0</v>
       </c>
-      <c r="K46" s="261" t="s">
+      <c r="K46" s="228" t="s">
         <v>120</v>
       </c>
-      <c r="L46" s="262" t="s">
+      <c r="L46" s="229" t="s">
         <v>52</v>
       </c>
       <c r="M46" s="169" t="s">
@@ -7091,54 +7218,54 @@
       <c r="N46" s="169" t="s">
         <v>37</v>
       </c>
-      <c r="O46" s="263" t="s">
-        <v>37</v>
-      </c>
-      <c r="P46" s="264"/>
-      <c r="Q46" s="264"/>
-      <c r="R46" s="264"/>
-      <c r="S46" s="264"/>
-      <c r="T46" s="264"/>
-      <c r="U46" s="265" t="s">
-        <v>52</v>
-      </c>
-      <c r="V46" s="266" t="s">
-        <v>37</v>
-      </c>
-      <c r="W46" s="267" t="s">
+      <c r="O46" s="230" t="s">
+        <v>37</v>
+      </c>
+      <c r="P46" s="231"/>
+      <c r="Q46" s="231"/>
+      <c r="R46" s="231"/>
+      <c r="S46" s="231"/>
+      <c r="T46" s="231"/>
+      <c r="U46" s="232" t="s">
+        <v>52</v>
+      </c>
+      <c r="V46" s="233" t="s">
+        <v>37</v>
+      </c>
+      <c r="W46" s="234" t="s">
         <v>4</v>
       </c>
-      <c r="X46" s="266" t="s">
+      <c r="X46" s="233" t="s">
         <v>2</v>
       </c>
-      <c r="Y46" s="266" t="s">
+      <c r="Y46" s="233" t="s">
         <v>2</v>
       </c>
-      <c r="Z46" s="267" t="s">
+      <c r="Z46" s="234" t="s">
         <v>2</v>
       </c>
-      <c r="AA46" s="268"/>
-      <c r="AB46" s="268"/>
-      <c r="AC46" s="268"/>
-      <c r="AD46" s="268"/>
-      <c r="AE46" s="268"/>
-      <c r="AF46" s="268"/>
-      <c r="AG46" s="268"/>
-      <c r="AH46" s="268"/>
-      <c r="AI46" s="268"/>
-      <c r="AJ46" s="268"/>
-      <c r="AK46" s="268"/>
-      <c r="AL46" s="269"/>
-      <c r="AM46" s="270" t="s">
+      <c r="AA46" s="235"/>
+      <c r="AB46" s="235"/>
+      <c r="AC46" s="235"/>
+      <c r="AD46" s="235"/>
+      <c r="AE46" s="235"/>
+      <c r="AF46" s="235"/>
+      <c r="AG46" s="235"/>
+      <c r="AH46" s="235"/>
+      <c r="AI46" s="235"/>
+      <c r="AJ46" s="235"/>
+      <c r="AK46" s="235"/>
+      <c r="AL46" s="236"/>
+      <c r="AM46" s="237" t="s">
         <v>73</v>
       </c>
-      <c r="AN46" s="271" t="s">
+      <c r="AN46" s="238" t="s">
         <v>208</v>
       </c>
-      <c r="AO46" s="272" t="s">
+      <c r="AO46" s="239" t="s">
         <v>209</v>
       </c>
-      <c r="AP46" s="273"/>
+      <c r="AP46" s="240"/>
     </row>
     <row r="47" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A47" s="84"/>

</xml_diff>

<commit_message>
Add logging to base page.
</commit_message>
<xml_diff>
--- a/proj02_springdemo/data/SpringDemo-MarketMatrix-20190517.xlsx
+++ b/proj02_springdemo/data/SpringDemo-MarketMatrix-20190517.xlsx
@@ -3227,11 +3227,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="10" ySplit="4" topLeftCell="K17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomRight" activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3250,7 +3250,9 @@
     <col min="13" max="13" width="25.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="25.140625" style="29" customWidth="1"/>
     <col min="16" max="20" width="25.140625" style="181" customWidth="1"/>
-    <col min="21" max="34" width="25.140625" style="29" customWidth="1"/>
+    <col min="21" max="31" width="25.140625" style="29" customWidth="1"/>
+    <col min="32" max="32" width="30.85546875" style="29" customWidth="1"/>
+    <col min="33" max="34" width="25.140625" style="29" customWidth="1"/>
     <col min="35" max="35" width="25.140625" style="82" customWidth="1"/>
     <col min="36" max="36" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="23.28515625" style="82" customWidth="1"/>
@@ -5436,7 +5438,7 @@
       <c r="AP25" s="27"/>
       <c r="AQ25" s="84"/>
     </row>
-    <row r="26" spans="1:43" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" s="22" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="158"/>
       <c r="B26" s="264"/>
       <c r="C26" s="271"/>
@@ -5496,8 +5498,8 @@
       <c r="AE26" s="195" t="s">
         <v>37</v>
       </c>
-      <c r="AF26" s="194" t="s">
-        <v>52</v>
+      <c r="AF26" s="116" t="s">
+        <v>37</v>
       </c>
       <c r="AG26" s="195" t="s">
         <v>37</v>
@@ -5561,8 +5563,8 @@
       <c r="N27" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="O27" s="170" t="s">
-        <v>52</v>
+      <c r="O27" s="149" t="s">
+        <v>37</v>
       </c>
       <c r="P27" s="37"/>
       <c r="Q27" s="37"/>
@@ -5650,8 +5652,8 @@
       <c r="N28" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="O28" s="170" t="s">
-        <v>52</v>
+      <c r="O28" s="149" t="s">
+        <v>37</v>
       </c>
       <c r="P28" s="37"/>
       <c r="Q28" s="37"/>
@@ -5739,8 +5741,8 @@
       <c r="N29" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="O29" s="170" t="s">
-        <v>52</v>
+      <c r="O29" s="149" t="s">
+        <v>37</v>
       </c>
       <c r="P29" s="37"/>
       <c r="Q29" s="37"/>
@@ -5826,8 +5828,8 @@
       <c r="N30" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="O30" s="170" t="s">
-        <v>52</v>
+      <c r="O30" s="149" t="s">
+        <v>37</v>
       </c>
       <c r="P30" s="37"/>
       <c r="Q30" s="37"/>
@@ -5913,8 +5915,8 @@
       <c r="N31" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="O31" s="170" t="s">
-        <v>52</v>
+      <c r="O31" s="149" t="s">
+        <v>37</v>
       </c>
       <c r="P31" s="37"/>
       <c r="Q31" s="37"/>
@@ -6000,8 +6002,8 @@
       <c r="N32" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="O32" s="170" t="s">
-        <v>52</v>
+      <c r="O32" s="149" t="s">
+        <v>37</v>
       </c>
       <c r="P32" s="37"/>
       <c r="Q32" s="37"/>
@@ -6087,8 +6089,8 @@
       <c r="N33" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="O33" s="170" t="s">
-        <v>52</v>
+      <c r="O33" s="149" t="s">
+        <v>37</v>
       </c>
       <c r="P33" s="37"/>
       <c r="Q33" s="37"/>
@@ -6174,8 +6176,8 @@
       <c r="N34" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="O34" s="170" t="s">
-        <v>52</v>
+      <c r="O34" s="149" t="s">
+        <v>37</v>
       </c>
       <c r="P34" s="37"/>
       <c r="Q34" s="37"/>
@@ -6263,8 +6265,8 @@
       <c r="N35" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="O35" s="170" t="s">
-        <v>52</v>
+      <c r="O35" s="149" t="s">
+        <v>37</v>
       </c>
       <c r="P35" s="37"/>
       <c r="Q35" s="37"/>
@@ -6352,8 +6354,8 @@
       <c r="N36" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="O36" s="170" t="s">
-        <v>52</v>
+      <c r="O36" s="149" t="s">
+        <v>37</v>
       </c>
       <c r="P36" s="37"/>
       <c r="Q36" s="37"/>
@@ -6441,8 +6443,8 @@
       <c r="N37" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="O37" s="170" t="s">
-        <v>52</v>
+      <c r="O37" s="149" t="s">
+        <v>37</v>
       </c>
       <c r="P37" s="37"/>
       <c r="Q37" s="37"/>
@@ -7364,7 +7366,7 @@
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O41 AI12 Y6:Z6 AK11 AA7:AH16 AL7:AL16 AJ7:AJ16 AL20:AL26 AJ20:AJ26 AA20:AH26 U17:V19 L27:N41 U27:V41 L17:N19 L5:N6 U5:V6 L42:V46">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA20:AH26 AI12 Y6:Z6 AK11 AA7:AH16 AL7:AL16 AJ7:AJ16 AL20:AL26 AJ20:AJ26 L42:V46 U17:V19 L27:N41 U27:V41 L17:N19 L5:N6 U5:V6 O5:O41">
       <formula1>"Please select, Yes, No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W6 W5:Z5 X18:Y18 W18:W19 Z18:Z19 W27:Z41 W46:Z46">

</xml_diff>